<commit_message>
Implement featured cell style when there is plantao date conflict
</commit_message>
<xml_diff>
--- a/testfiles/entrada/template_HistoricoAfastamento.xlsx
+++ b/testfiles/entrada/template_HistoricoAfastamento.xlsx
@@ -14,6 +14,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Page 1'!$A$1:$T$33</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Page 1'!$A$1:$T$33</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Page 1'!$A$1:$T$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Page 1'!$A$1:$T$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Page 1'!$A$1:$T$33</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="151">
   <si>
     <t xml:space="preserve">HEADER 01</t>
   </si>
@@ -165,6 +167,12 @@
     <t xml:space="preserve">Sim</t>
   </si>
   <si>
+    <t xml:space="preserve">04/01/2017 00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2017 00:00:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">06/06/2018 00:00:00</t>
   </si>
   <si>
@@ -184,6 +192,12 @@
   </si>
   <si>
     <t xml:space="preserve">LICENCA PARA TRATAMENTO DE SAUDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2017 00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/01/2017 00:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">12/06/2018 00:00:00</t>
@@ -769,32 +783,31 @@
   <dimension ref="A1:T65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="46.1683673469388"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="48.1938775510204"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="0.943877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="48.4642857142857"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="115.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="112.719387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -992,37 +1005,37 @@
     </row>
     <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G11" s="9" t="n">
         <v>12332165480</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>41</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>44</v>
@@ -1051,37 +1064,37 @@
     </row>
     <row r="12" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G12" s="9" t="n">
         <v>12332165481</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L12" s="11" t="s">
         <v>44</v>
@@ -1114,25 +1127,25 @@
         <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G13" s="9" t="n">
         <v>12332165482</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>29</v>
@@ -1164,34 +1177,34 @@
         <v>22</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G14" s="9" t="n">
         <v>12332165483</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>44</v>
@@ -1221,37 +1234,37 @@
     </row>
     <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="F15" s="9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G15" s="9" t="n">
         <v>12332165484</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>41</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>44</v>
@@ -1280,28 +1293,28 @@
     </row>
     <row r="16" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>12332165485</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="K16" s="11" t="s">
         <v>28</v>
@@ -1334,25 +1347,25 @@
     </row>
     <row r="17" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>12332165486</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>28</v>
@@ -1384,28 +1397,28 @@
     </row>
     <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G18" s="9" t="n">
         <v>12332165487</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K18" s="11" t="s">
         <v>28</v>
@@ -1438,37 +1451,37 @@
     </row>
     <row r="19" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>12332165488</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L19" s="9" t="s">
         <v>44</v>
@@ -1497,37 +1510,37 @@
     </row>
     <row r="20" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>12332165489</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L20" s="11" t="s">
         <v>44</v>
@@ -1557,7 +1570,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>22</v>
@@ -1566,28 +1579,28 @@
         <v>22</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G21" s="9" t="n">
         <v>12332165490</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="L21" s="9" t="s">
         <v>44</v>
@@ -1616,34 +1629,34 @@
     </row>
     <row r="22" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>38</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G22" s="9" t="n">
         <v>12332165491</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="K22" s="11" t="s">
         <v>43</v>
@@ -1676,37 +1689,37 @@
     </row>
     <row r="23" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G23" s="9" t="n">
         <v>12332165492</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>41</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L23" s="9" t="s">
         <v>44</v>
@@ -1735,37 +1748,37 @@
     </row>
     <row r="24" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G24" s="9" t="n">
         <v>12332165493</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L24" s="11" t="s">
         <v>44</v>
@@ -1795,37 +1808,37 @@
     </row>
     <row r="25" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G25" s="9" t="n">
         <v>12332165494</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>41</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L25" s="9" t="s">
         <v>44</v>
@@ -1854,37 +1867,37 @@
     </row>
     <row r="26" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G26" s="9" t="n">
         <v>12332165495</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>44</v>
@@ -1914,37 +1927,37 @@
     </row>
     <row r="27" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G27" s="9" t="n">
         <v>12332165496</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L27" s="9" t="s">
         <v>44</v>
@@ -1973,37 +1986,37 @@
     </row>
     <row r="28" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G28" s="9" t="n">
         <v>12332165497</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L28" s="11" t="s">
         <v>44</v>
@@ -2034,7 +2047,7 @@
     <row r="29" customFormat="false" ht="2.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -2056,7 +2069,7 @@
     </row>
     <row r="31" customFormat="false" ht="11.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2078,7 +2091,7 @@
     </row>
     <row r="32" customFormat="false" ht="2.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>

</xml_diff>